<commit_message>
agregar los valores de la venta actual
</commit_message>
<xml_diff>
--- a/Internacional/Inputs/Parametros.xlsx
+++ b/Internacional/Inputs/Parametros.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsilva\Documents\Tiara Silva\Proyecciones-S-OP\Internacional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiarasilva/Documents/2022-S2/Práctica II/Agrosuper/Proyecciones/Proyecciones-S-OP/Internacional/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246DB162-765F-4375-8E41-E950D1FE4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D697B4B-26CF-6C4E-AE48-D35A1CCC469E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29700" windowHeight="15000" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead time" sheetId="1" r:id="rId1"/>
     <sheet name="Venta" sheetId="3" r:id="rId2"/>
     <sheet name="Criterios" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Oficina</t>
   </si>
@@ -118,7 +118,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,19 +141,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -510,7 +517,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -527,81 +534,92 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0] 3" xfId="2" xr:uid="{B8A90921-2E36-4D30-8A52-9EB0BD1901AA}"/>
@@ -622,7 +640,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -910,7 +928,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -918,335 +936,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAEE0AC-A22C-D142-BF90-0F0256C89132}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="7" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="8" t="s">
+      <c r="B2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="23">
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="D2" s="24">
+        <v>7</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28">
+        <f t="shared" ref="H2:H6" si="0">SUM(C2:D2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="23">
+        <v>3.0034758973294529</v>
+      </c>
+      <c r="D3" s="24">
+        <v>7</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28">
+        <f t="shared" si="0"/>
+        <v>10.003475897329453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="23">
+        <v>4.657346307107681</v>
+      </c>
+      <c r="D4" s="24">
+        <v>7</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28">
+        <f t="shared" si="0"/>
+        <v>11.65734630710768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8" t="s">
+      <c r="C5" s="23">
+        <v>4.2658490213417863</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28">
+        <f t="shared" si="0"/>
+        <v>4.2658490213417863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="33">
+        <v>5.0000000000000027</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="39">
         <v>1.7096242985822629</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="39">
         <v>7</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="39">
         <v>34.12185483870968</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="39">
         <v>7.5</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="39">
         <v>9.5</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="40">
         <f>SUM(C7:G7)</f>
         <v>59.831479137291943</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="42">
         <v>7.1716200124743272</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="39">
         <v>7</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="42">
         <v>42.5</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="42">
         <v>5.1420118343195265</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="42">
         <v>7.5</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="43">
         <f>SUM(C8:G8)</f>
         <v>69.313631846793854</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="25" t="s">
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="42">
         <v>2.1855088411235015</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="39">
         <v>7</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="42">
         <v>15.041530944625407</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="42">
         <v>5.4496124031007751</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="42">
         <v>10</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="43">
         <f>SUM(C9:G9)</f>
         <v>39.676652188849687</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="42">
         <v>4.7953843510197851</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="39">
         <v>7</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="42">
         <v>44.199230302961368</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="42">
         <v>5.5741092456127026</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="42">
         <v>5.5</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="43">
         <f>SUM(C10:G10)</f>
         <v>67.068723899593863</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="26" t="s">
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="45">
         <v>5.0102395291990982</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="39">
         <v>7</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="45">
         <v>35.255201787459853</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="45">
         <v>4.830303030303031</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="45">
         <v>15</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="46">
         <f>SUM(C11:G11)</f>
         <v>67.095744346961979</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="29">
-        <v>3.0000000000000004</v>
-      </c>
-      <c r="D14" s="30">
-        <v>7</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34">
-        <f t="shared" ref="H14:H18" si="0">SUM(C14:D14)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="29">
-        <v>3.0034758973294529</v>
-      </c>
-      <c r="D15" s="30">
-        <v>7</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34">
-        <f t="shared" si="0"/>
-        <v>10.003475897329453</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="29">
-        <v>4.657346307107681</v>
-      </c>
-      <c r="D16" s="30">
-        <v>7</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34">
-        <f t="shared" si="0"/>
-        <v>11.65734630710768</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="29">
-        <v>4.2658490213417863</v>
-      </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34">
-        <f t="shared" si="0"/>
-        <v>4.2658490213417863</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="36">
-        <v>5.0000000000000027</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000027</v>
-      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1262,13 +1224,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
@@ -1284,31 +1246,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA9B73F-3FB7-489E-971B-CBC65E0FD9A6}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="258" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1284,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="8" t="s">
         <v>3</v>
@@ -1330,7 +1292,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="8" t="s">
         <v>4</v>
@@ -1338,7 +1300,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
@@ -1346,7 +1308,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="9" t="s">
         <v>6</v>
@@ -1354,7 +1316,7 @@
       <c r="C6" s="9"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1364,7 +1326,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
@@ -1372,7 +1334,7 @@
       <c r="C8" s="8"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="8" t="s">
         <v>2</v>
@@ -1380,7 +1342,7 @@
       <c r="C9" s="8"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="8" t="s">
         <v>10</v>
@@ -1388,7 +1350,7 @@
       <c r="C10" s="8"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="8" t="s">
         <v>11</v>
@@ -1396,7 +1358,7 @@
       <c r="C11" s="8"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="9" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
add message box, upgrade proyection by time
</commit_message>
<xml_diff>
--- a/Internacional/Inputs/Parametros.xlsx
+++ b/Internacional/Inputs/Parametros.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiarasilva/Documents/2022-S2/Práctica II/Agrosuper/Proyecciones/Proyecciones-S-OP/Internacional/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D697B4B-26CF-6C4E-AE48-D35A1CCC469E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA675FE-0565-D042-9B37-150627826D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29700" windowHeight="15000" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23460" windowHeight="18080" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lead time" sheetId="1" r:id="rId1"/>
-    <sheet name="Venta" sheetId="3" r:id="rId2"/>
-    <sheet name="Criterios" sheetId="4" r:id="rId3"/>
+    <sheet name="Lead time" sheetId="5" r:id="rId1"/>
+    <sheet name="Cierre venta" sheetId="6" r:id="rId2"/>
+    <sheet name="Lead time 2" sheetId="1" r:id="rId3"/>
+    <sheet name="Venta" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>Oficina</t>
   </si>
@@ -80,21 +81,9 @@
     <t>Tipo de venta</t>
   </si>
   <si>
-    <t>Semanas</t>
-  </si>
-  <si>
-    <t>Criterio n + 1</t>
-  </si>
-  <si>
-    <t>Criterio n + 2</t>
-  </si>
-  <si>
     <t>Tipo de venta seleccionada</t>
   </si>
   <si>
-    <t>Directa</t>
-  </si>
-  <si>
     <t>Planta</t>
   </si>
   <si>
@@ -108,6 +97,90 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mes seleccionado </t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>* Hasta el 15 del mes</t>
+  </si>
+  <si>
+    <t>* Hasta el 12 se va a facturar durante el mes</t>
+  </si>
+  <si>
+    <t>* Hasta el 20</t>
+  </si>
+  <si>
+    <t>60% se va a vender para n+1</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>40% se va vender para n+2</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>n+1</t>
+  </si>
+  <si>
+    <t>Considerando días hábiles</t>
+  </si>
+  <si>
+    <t>Sin días hábiles</t>
+  </si>
+  <si>
+    <t>Máx días</t>
+  </si>
+  <si>
+    <t>Mín días</t>
+  </si>
+  <si>
+    <t>Solo domingos</t>
+  </si>
+  <si>
+    <t>Mes n</t>
+  </si>
+  <si>
+    <t>Mes n + 1</t>
+  </si>
+  <si>
+    <t>Mes n + 2</t>
+  </si>
+  <si>
+    <t>n+2</t>
+  </si>
+  <si>
+    <t>n+3</t>
+  </si>
+  <si>
+    <t>Almacen</t>
+  </si>
+  <si>
+    <t>Puerto Oficina</t>
+  </si>
+  <si>
+    <t>Porcentaje de producción</t>
+  </si>
+  <si>
+    <t>Porcentaje de asignación mes n+2</t>
+  </si>
+  <si>
+    <t>OPTIMISTA</t>
+  </si>
+  <si>
+    <t>PESIMISTA</t>
   </si>
 </sst>
 </file>
@@ -118,7 +191,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,8 +237,51 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +305,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -265,17 +397,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -286,30 +407,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -511,46 +608,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -560,39 +707,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -601,27 +763,70 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="20% - Énfasis4" xfId="5" builtinId="42"/>
+    <cellStyle name="Bueno" xfId="3" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="4" builtinId="27"/>
     <cellStyle name="Millares [0] 3" xfId="2" xr:uid="{B8A90921-2E36-4D30-8A52-9EB0BD1901AA}"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +845,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -928,18 +1133,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAEE0AC-A22C-D142-BF90-0F0256C89132}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42CA654-57D7-6644-B2CE-03B9B53FD56F}">
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,263 +1157,498 @@
     <col min="6" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="10">
         <v>3.0000000000000004</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="10">
         <v>7</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28">
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14">
         <f t="shared" ref="H2:H6" si="0">SUM(C2:D2)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="56"/>
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="10">
         <v>3.0034758973294529</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="28">
         <v>7</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28">
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14">
         <f t="shared" si="0"/>
         <v>10.003475897329453</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="10">
         <v>4.657346307107681</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="28">
         <v>7</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28">
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14">
         <f t="shared" si="0"/>
         <v>11.65734630710768</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="10">
         <v>4.2658490213417863</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28">
+      <c r="D5" s="28"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14">
         <f t="shared" si="0"/>
         <v>4.2658490213417863</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="57"/>
+      <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="19">
         <v>5.0000000000000027</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37">
+      <c r="D6" s="31"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23">
         <f t="shared" si="0"/>
         <v>5.0000000000000027</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="25">
         <v>1.7096242985822629</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="25">
         <v>7</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="25">
         <v>34.12185483870968</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="25">
         <v>7.5</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="25">
         <v>9.5</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="26">
         <f>SUM(C7:G7)</f>
         <v>59.831479137291943</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="41" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="56"/>
+      <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="28">
         <v>7.1716200124743272</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="28">
         <v>7</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="28">
         <v>42.5</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="28">
         <v>5.1420118343195265</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="28">
         <v>7.5</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="29">
         <f>SUM(C8:G8)</f>
         <v>69.313631846793854</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="41" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="56"/>
+      <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="28">
         <v>2.1855088411235015</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="28">
         <v>7</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="28">
         <v>15.041530944625407</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="28">
         <v>5.4496124031007751</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="28">
         <v>10</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="29">
         <f>SUM(C9:G9)</f>
         <v>39.676652188849687</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="41" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="56"/>
+      <c r="B10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="28">
         <v>4.7953843510197851</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="28">
         <v>7</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="28">
         <v>44.199230302961368</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="28">
         <v>5.5741092456127026</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="28">
         <v>5.5</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="29">
         <f>SUM(C10:G10)</f>
         <v>67.068723899593863</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="57"/>
+      <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="31">
         <v>5.0102395291990982</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="31">
         <v>7</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="31">
         <v>35.255201787459853</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="31">
         <v>4.830303030303031</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="31">
         <v>15</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="32">
         <f>SUM(C11:G11)</f>
         <v>67.095744346961979</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10">
+        <f>C2+$J$19</f>
+        <v>5</v>
+      </c>
+      <c r="D14" s="10">
+        <f>D2+$J$19</f>
+        <v>9</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14">
+        <f t="shared" ref="H14:H18" si="1">SUM(C14:D14)</f>
         <v>14</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10">
+        <f>C3+$J$19</f>
+        <v>5.0034758973294533</v>
+      </c>
+      <c r="D15" s="10">
+        <f>D3+$J$19</f>
+        <v>9</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14">
+        <f t="shared" si="1"/>
+        <v>14.003475897329453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="10">
+        <f>C4+$J$19</f>
+        <v>6.657346307107681</v>
+      </c>
+      <c r="D16" s="10">
+        <f>D4+$J$19</f>
+        <v>9</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14">
+        <f t="shared" si="1"/>
+        <v>15.65734630710768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10">
+        <f>C5+$J$19</f>
+        <v>6.2658490213417863</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14">
+        <f t="shared" si="1"/>
+        <v>6.2658490213417863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="10">
+        <f>C6+$J$19</f>
+        <v>7.0000000000000027</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25">
+        <f>F7+$J$19</f>
+        <v>9.5</v>
+      </c>
+      <c r="G19" s="25">
+        <f>G7+$J$19</f>
+        <v>11.5</v>
+      </c>
+      <c r="H19" s="26">
+        <f>SUM(C19:G19)</f>
+        <v>21</v>
+      </c>
+      <c r="J19" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28">
+        <f>F8+$J$19</f>
+        <v>7.1420118343195265</v>
+      </c>
+      <c r="G20" s="28">
+        <f>G8+$J$19</f>
+        <v>9.5</v>
+      </c>
+      <c r="H20" s="29">
+        <f>SUM(C20:G20)</f>
+        <v>16.642011834319526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28">
+        <f>F9+$J$19</f>
+        <v>7.4496124031007751</v>
+      </c>
+      <c r="G21" s="28">
+        <f>G9+$J$19</f>
+        <v>12</v>
+      </c>
+      <c r="H21" s="29">
+        <f>SUM(C21:G21)</f>
+        <v>19.449612403100776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28">
+        <f>F10+$J$19</f>
+        <v>7.5741092456127026</v>
+      </c>
+      <c r="G22" s="28">
+        <f>G10+$J$19</f>
+        <v>7.5</v>
+      </c>
+      <c r="H22" s="29">
+        <f>SUM(C22:G22)</f>
+        <v>15.074109245612703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31">
+        <f>F11+$J$19</f>
+        <v>6.830303030303031</v>
+      </c>
+      <c r="G23" s="31">
+        <f>G11+$J$19</f>
+        <v>17</v>
+      </c>
+      <c r="H23" s="32">
+        <f>SUM(C23:G23)</f>
+        <v>23.830303030303032</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1217,24 +1657,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D451A9-327B-1444-822B-9D6B797FC747}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A755B6F-994F-7F4A-BED3-8439B833EF15}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="169" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="31">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1243,128 +1781,715 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA9B73F-3FB7-489E-971B-CBC65E0FD9A6}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAEE0AC-A22C-D142-BF90-0F0256C89132}">
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="258" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="10">
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="E2" s="10">
+        <v>7</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14">
+        <f t="shared" ref="I2:I6" si="0">SUM(D2:E2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="10">
+        <v>3.0034758973294529</v>
+      </c>
+      <c r="E3" s="28">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14">
+        <f t="shared" si="0"/>
+        <v>10.003475897329453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="10">
+        <v>4.657346307107681</v>
+      </c>
+      <c r="E4" s="28">
+        <v>7</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>11.65734630710768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="10">
+        <v>4.2658490213417863</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14">
+        <f t="shared" si="0"/>
+        <v>4.2658490213417863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="19">
+        <v>5.0000000000000027</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1.7096242985822629</v>
+      </c>
+      <c r="E7" s="25">
+        <v>7</v>
+      </c>
+      <c r="F7" s="25">
+        <v>34.12185483870968</v>
+      </c>
+      <c r="G7" s="25">
+        <v>7.5</v>
+      </c>
+      <c r="H7" s="25">
+        <v>9.5</v>
+      </c>
+      <c r="I7" s="14">
+        <f>SUM(D7:H7)</f>
+        <v>59.831479137291943</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="28">
+        <v>7.1716200124743272</v>
+      </c>
+      <c r="E8" s="28">
+        <v>7</v>
+      </c>
+      <c r="F8" s="28">
+        <v>42.5</v>
+      </c>
+      <c r="G8" s="28">
+        <v>5.1420118343195265</v>
+      </c>
+      <c r="H8" s="28">
+        <v>7.5</v>
+      </c>
+      <c r="I8" s="14">
+        <f>SUM(D8:H8)</f>
+        <v>69.313631846793854</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="28">
+        <v>2.1855088411235015</v>
+      </c>
+      <c r="E9" s="28">
+        <v>7</v>
+      </c>
+      <c r="F9" s="28">
+        <v>15.041530944625407</v>
+      </c>
+      <c r="G9" s="28">
+        <v>5.4496124031007751</v>
+      </c>
+      <c r="H9" s="28">
+        <v>10</v>
+      </c>
+      <c r="I9" s="14">
+        <f>SUM(D9:H9)</f>
+        <v>39.676652188849687</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="28">
+        <v>4.7953843510197851</v>
+      </c>
+      <c r="E10" s="28">
+        <v>7</v>
+      </c>
+      <c r="F10" s="28">
+        <v>44.199230302961368</v>
+      </c>
+      <c r="G10" s="28">
+        <v>5.5741092456127026</v>
+      </c>
+      <c r="H10" s="28">
+        <v>5.5</v>
+      </c>
+      <c r="I10" s="14">
+        <f>SUM(D10:H10)</f>
+        <v>67.068723899593863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="31">
+        <v>5.0102395291990982</v>
+      </c>
+      <c r="E11" s="31">
+        <v>7</v>
+      </c>
+      <c r="F11" s="31">
+        <v>35.255201787459853</v>
+      </c>
+      <c r="G11" s="31">
+        <v>4.830303030303031</v>
+      </c>
+      <c r="H11" s="31">
+        <v>15</v>
+      </c>
+      <c r="I11" s="23">
+        <f>SUM(D11:H11)</f>
+        <v>67.095744346961979</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="41">
+        <f>SUM(D7:H7)</f>
+        <v>59.831479137291943</v>
+      </c>
+      <c r="E12" s="41">
+        <f>SUM(E7:H7)</f>
+        <v>58.12185483870968</v>
+      </c>
+      <c r="F12" s="41">
+        <f>SUM(F7:H7)</f>
+        <v>51.12185483870968</v>
+      </c>
+      <c r="G12" s="40">
+        <f>G7+H7</f>
+        <v>17</v>
+      </c>
+      <c r="H12" s="40">
+        <f>H7</f>
+        <v>9.5</v>
+      </c>
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="49"/>
+      <c r="C13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="42">
+        <f>SUM(D8:H8)</f>
+        <v>69.313631846793854</v>
+      </c>
+      <c r="E13" s="42">
+        <f>SUM(E8:H8)</f>
+        <v>62.142011834319526</v>
+      </c>
+      <c r="F13" s="41">
+        <f>SUM(F8:H8)</f>
+        <v>55.142011834319526</v>
+      </c>
+      <c r="G13" s="40">
+        <f>G8+H8</f>
+        <v>12.642011834319526</v>
+      </c>
+      <c r="H13" s="40">
+        <f>H8</f>
+        <v>7.5</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="49"/>
+      <c r="C14" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="41">
+        <f t="shared" ref="D14:D16" si="1">SUM(D9:H9)</f>
+        <v>39.676652188849687</v>
+      </c>
+      <c r="E14" s="41">
+        <f>SUM(E9:H9)</f>
+        <v>37.49114334772618</v>
+      </c>
+      <c r="F14" s="40">
+        <f t="shared" ref="F14:F16" si="2">SUM(F9:H9)</f>
+        <v>30.491143347726183</v>
+      </c>
+      <c r="G14" s="40">
+        <f t="shared" ref="G14:G16" si="3">G9+H9</f>
+        <v>15.449612403100776</v>
+      </c>
+      <c r="H14" s="40">
+        <f t="shared" ref="H14:H16" si="4">H9</f>
+        <v>10</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="49"/>
+      <c r="C15" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="42">
+        <f t="shared" si="1"/>
+        <v>67.068723899593863</v>
+      </c>
+      <c r="E15" s="42">
+        <f>SUM(E10:H10)</f>
+        <v>62.273339548574072</v>
+      </c>
+      <c r="F15" s="41">
+        <f t="shared" si="2"/>
+        <v>55.273339548574072</v>
+      </c>
+      <c r="G15" s="40">
+        <f t="shared" si="3"/>
+        <v>11.074109245612703</v>
+      </c>
+      <c r="H15" s="40">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="49"/>
+      <c r="C16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="42">
+        <f t="shared" si="1"/>
+        <v>67.095744346961979</v>
+      </c>
+      <c r="E16" s="42">
+        <f>SUM(E11:H11)</f>
+        <v>62.085504817762882</v>
+      </c>
+      <c r="F16" s="41">
+        <f t="shared" si="2"/>
+        <v>55.085504817762882</v>
+      </c>
+      <c r="G16" s="40">
+        <f t="shared" si="3"/>
+        <v>19.830303030303032</v>
+      </c>
+      <c r="H16" s="40">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+    </row>
+    <row r="18" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="42">
+        <f>SUM(D7:H7)</f>
+        <v>59.831479137291943</v>
+      </c>
+      <c r="E19" s="42">
+        <f>SUM(E7:H7)</f>
+        <v>58.12185483870968</v>
+      </c>
+      <c r="F19" s="41">
+        <f>SUM(F7:H7)</f>
+        <v>51.12185483870968</v>
+      </c>
+      <c r="G19" s="40">
+        <f>SUM(G7:H7)</f>
+        <v>17</v>
+      </c>
+      <c r="H19" s="40">
+        <f>H7</f>
+        <v>9.5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19">
+        <f>31 - 4</f>
+        <v>27</v>
+      </c>
+      <c r="L19">
+        <f>K19*2</f>
+        <v>54</v>
+      </c>
+      <c r="M19">
+        <f>K19*3</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="54"/>
+      <c r="C20" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="42">
+        <f>SUM(D8:H8)</f>
+        <v>69.313631846793854</v>
+      </c>
+      <c r="E20" s="42">
+        <f>SUM(E8:H8)</f>
+        <v>62.142011834319526</v>
+      </c>
+      <c r="F20" s="42">
+        <f>SUM(F8:H8)</f>
+        <v>55.142011834319526</v>
+      </c>
+      <c r="G20" s="40">
+        <f>SUM(G8:H8)</f>
+        <v>12.642011834319526</v>
+      </c>
+      <c r="H20" s="40">
+        <f>H8</f>
+        <v>7.5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20">
+        <f>28-4</f>
+        <v>24</v>
+      </c>
+      <c r="L20">
+        <f>K20*2</f>
+        <v>48</v>
+      </c>
+      <c r="M20">
+        <f>K20*3</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="54"/>
+      <c r="C21" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="41">
+        <f t="shared" ref="D21:D23" si="5">SUM(D9:H9)</f>
+        <v>39.676652188849687</v>
+      </c>
+      <c r="E21" s="41">
+        <f t="shared" ref="E21:E23" si="6">SUM(E9:H9)</f>
+        <v>37.49114334772618</v>
+      </c>
+      <c r="F21" s="41">
+        <f t="shared" ref="F21:F23" si="7">SUM(F9:H9)</f>
+        <v>30.491143347726183</v>
+      </c>
+      <c r="G21" s="40">
+        <f t="shared" ref="G21:G23" si="8">SUM(G9:H9)</f>
+        <v>15.449612403100776</v>
+      </c>
+      <c r="H21" s="40">
+        <f t="shared" ref="H21:H23" si="9">H9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="54"/>
+      <c r="C22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="42">
+        <f t="shared" si="5"/>
+        <v>67.068723899593863</v>
+      </c>
+      <c r="E22" s="42">
+        <f t="shared" si="6"/>
+        <v>62.273339548574072</v>
+      </c>
+      <c r="F22" s="42">
+        <f t="shared" si="7"/>
+        <v>55.273339548574072</v>
+      </c>
+      <c r="G22" s="40">
+        <f t="shared" si="8"/>
+        <v>11.074109245612703</v>
+      </c>
+      <c r="H22" s="40">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="42">
+        <f t="shared" si="5"/>
+        <v>67.095744346961979</v>
+      </c>
+      <c r="E23" s="42">
+        <f t="shared" si="6"/>
+        <v>62.085504817762882</v>
+      </c>
+      <c r="F23" s="42">
+        <f t="shared" si="7"/>
+        <v>55.085504817762882</v>
+      </c>
+      <c r="G23" s="40">
+        <f t="shared" si="8"/>
+        <v>19.830303030303032</v>
+      </c>
+      <c r="H23" s="40">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="50"/>
+      <c r="C27" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="50"/>
+      <c r="C28" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="50"/>
+      <c r="C29" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+      <c r="C30" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B19:B23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D451A9-327B-1444-822B-9D6B797FC747}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="45">
+        <v>0.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add file of pivot table
</commit_message>
<xml_diff>
--- a/Internacional/Inputs/Parametros.xlsx
+++ b/Internacional/Inputs/Parametros.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiarasilva/Documents/2022-S2/Práctica II/Agrosuper/Proyecciones/Proyecciones-S-OP/Internacional/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA675FE-0565-D042-9B37-150627826D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2120FCC2-9EE9-E846-986C-3F51AEF5CDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23460" windowHeight="18080" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" activeTab="4" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead time" sheetId="5" r:id="rId1"/>
     <sheet name="Cierre venta" sheetId="6" r:id="rId2"/>
     <sheet name="Lead time 2" sheetId="1" r:id="rId3"/>
     <sheet name="Venta" sheetId="3" r:id="rId4"/>
+    <sheet name="Asignación productivo" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="48">
   <si>
     <t>Oficina</t>
   </si>
@@ -677,15 +678,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -798,38 +800,45 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="17" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Énfasis4" xfId="5" builtinId="42"/>
     <cellStyle name="Bueno" xfId="3" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="4" builtinId="27"/>
     <cellStyle name="Millares [0] 3" xfId="2" xr:uid="{B8A90921-2E36-4D30-8A52-9EB0BD1901AA}"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1143,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42CA654-57D7-6644-B2CE-03B9B53FD56F}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1184,7 +1193,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1205,7 +1214,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="56"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1233,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="56"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1252,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="56"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1269,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1286,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="48" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -1304,7 +1313,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="56"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1338,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1363,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="56"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="27" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1388,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
@@ -1447,18 +1456,18 @@
         <v>12</v>
       </c>
       <c r="C14" s="10">
-        <f>C2+$J$19</f>
+        <f t="shared" ref="C14:D16" si="1">C2+$J$19</f>
         <v>5</v>
       </c>
       <c r="D14" s="10">
-        <f>D2+$J$19</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14">
-        <f t="shared" ref="H14:H18" si="1">SUM(C14:D14)</f>
+        <f t="shared" ref="H14:H18" si="2">SUM(C14:D14)</f>
         <v>14</v>
       </c>
     </row>
@@ -1468,18 +1477,18 @@
         <v>5</v>
       </c>
       <c r="C15" s="10">
-        <f>C3+$J$19</f>
+        <f t="shared" si="1"/>
         <v>5.0034758973294533</v>
       </c>
       <c r="D15" s="10">
-        <f>D3+$J$19</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.003475897329453</v>
       </c>
     </row>
@@ -1489,18 +1498,18 @@
         <v>6</v>
       </c>
       <c r="C16" s="10">
-        <f>C4+$J$19</f>
+        <f t="shared" si="1"/>
         <v>6.657346307107681</v>
       </c>
       <c r="D16" s="10">
-        <f>D4+$J$19</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.65734630710768</v>
       </c>
     </row>
@@ -1518,7 +1527,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2658490213417863</v>
       </c>
     </row>
@@ -1536,7 +1545,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="H18" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0000000000000027</v>
       </c>
     </row>
@@ -1551,11 +1560,11 @@
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25">
-        <f>F7+$J$19</f>
+        <f t="shared" ref="F19:G23" si="3">F7+$J$19</f>
         <v>9.5</v>
       </c>
       <c r="G19" s="25">
-        <f>G7+$J$19</f>
+        <f t="shared" si="3"/>
         <v>11.5</v>
       </c>
       <c r="H19" s="26">
@@ -1575,11 +1584,11 @@
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28">
-        <f>F8+$J$19</f>
+        <f t="shared" si="3"/>
         <v>7.1420118343195265</v>
       </c>
       <c r="G20" s="28">
-        <f>G8+$J$19</f>
+        <f t="shared" si="3"/>
         <v>9.5</v>
       </c>
       <c r="H20" s="29">
@@ -1596,11 +1605,11 @@
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28">
-        <f>F9+$J$19</f>
+        <f t="shared" si="3"/>
         <v>7.4496124031007751</v>
       </c>
       <c r="G21" s="28">
-        <f>G9+$J$19</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H21" s="29">
@@ -1617,11 +1626,11 @@
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28">
-        <f>F10+$J$19</f>
+        <f t="shared" si="3"/>
         <v>7.5741092456127026</v>
       </c>
       <c r="G22" s="28">
-        <f>G10+$J$19</f>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="H22" s="29">
@@ -1638,11 +1647,11 @@
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31">
-        <f>F11+$J$19</f>
+        <f t="shared" si="3"/>
         <v>6.830303030303031</v>
       </c>
       <c r="G23" s="31">
-        <f>G11+$J$19</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="H23" s="32">
@@ -1661,7 +1670,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="169" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,7 +1793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAEE0AC-A22C-D142-BF90-0F0256C89132}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2070,7 +2079,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="33"/>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="53" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -2099,7 +2108,7 @@
       <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="27" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2137,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="49"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="27" t="s">
         <v>2</v>
       </c>
@@ -2157,7 +2166,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="49"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="27" t="s">
         <v>11</v>
       </c>
@@ -2186,7 +2195,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="49"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="30" t="s">
         <v>8</v>
       </c>
@@ -2218,11 +2227,11 @@
       <c r="H17" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="53" t="s">
+      <c r="K17" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
     </row>
     <row r="18" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K18" s="43" t="s">
@@ -2236,7 +2245,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="59" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="24" t="s">
@@ -2279,7 +2288,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="54"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="27" t="s">
         <v>9</v>
       </c>
@@ -2320,7 +2329,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="54"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="27" t="s">
         <v>2</v>
       </c>
@@ -2346,7 +2355,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="54"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="27" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2381,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="30" t="s">
         <v>8</v>
       </c>
@@ -2399,7 +2408,7 @@
     </row>
     <row r="25" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="55" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="24" t="s">
@@ -2407,35 +2416,35 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="50"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="50"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52" t="s">
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B29" s="50"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="30" t="s">
         <v>8</v>
       </c>
@@ -2494,4 +2503,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6338382-DA91-DA4E-9040-DF0B4A9020DB}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="51">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="51">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="51">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="52">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying to work with exe fileÂ
</commit_message>
<xml_diff>
--- a/Internacional/Inputs/Parametros.xlsx
+++ b/Internacional/Inputs/Parametros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiarasilva/Documents/2022-S2/Práctica II/Agrosuper/Proyecciones/Proyecciones-S-OP/Internacional/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiarasilva/Documents/2022-S2/Práctica II/Agrosuper/Proyecciones/Proyecciones-S-OP/Internacional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2120FCC2-9EE9-E846-986C-3F51AEF5CDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BAC569-4278-CC40-AE69-5403A216223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" activeTab="4" xr2:uid="{D059D8C6-2807-D449-9D92-9DC1313178D6}"/>
   </bookViews>

</xml_diff>